<commit_message>
the users can now import sheets of contacts
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\resurse CRM\Aplicatie licenta 2023 - 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA96ED15-8C26-4DEE-8A39-CCB27515CEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81031DD-E084-4224-915D-5D007054D2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B355F5BB-8E75-495C-9323-1289A2C9F933}"/>
   </bookViews>
@@ -137,9 +137,6 @@
     <t>awd3r3r</t>
   </si>
   <si>
-    <t>adw3</t>
-  </si>
-  <si>
     <t>lead</t>
   </si>
   <si>
@@ -204,13 +201,16 @@
   </si>
   <si>
     <t>‎robertutzu_cs12@​yahoo.com</t>
+  </si>
+  <si>
+    <t>adw3@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -222,6 +222,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -271,15 +279,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -718,40 +729,40 @@
       <c r="C4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>12</v>
@@ -762,7 +773,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
@@ -771,7 +782,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>12</v>
@@ -783,7 +794,7 @@
         <v>12</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -791,13 +802,13 @@
         <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D7" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>14</v>
@@ -814,16 +825,16 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>16</v>
@@ -840,16 +851,16 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>18</v>
@@ -875,7 +886,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>19</v>
@@ -892,16 +903,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>20</v>
@@ -918,16 +929,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>12</v>
@@ -943,6 +954,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D4" r:id="rId1" xr:uid="{BBFBC5B6-90FD-4B47-8A56-75B5569ED354}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more phone number validation
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\resurse CRM\Aplicatie licenta 2023 - 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81031DD-E084-4224-915D-5D007054D2AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03DC2278-FEC8-4612-8C3C-E43ED5B19DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B355F5BB-8E75-495C-9323-1289A2C9F933}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
   <si>
     <t>firstName</t>
   </si>
@@ -204,6 +204,27 @@
   </si>
   <si>
     <t>adw3@gmail.com</t>
+  </si>
+  <si>
+    <t>0765893872</t>
+  </si>
+  <si>
+    <t>0721748392</t>
+  </si>
+  <si>
+    <t>+40765126291</t>
+  </si>
+  <si>
+    <t>+765472891</t>
+  </si>
+  <si>
+    <t>0721745592</t>
+  </si>
+  <si>
+    <t>0712348392</t>
+  </si>
+  <si>
+    <t>0721799423</t>
   </si>
 </sst>
 </file>
@@ -283,11 +304,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -626,7 +648,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,8 +705,8 @@
       <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="2">
-        <v>765893872</v>
+      <c r="F2" s="4" t="s">
+        <v>56</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>9</v>
@@ -709,8 +731,8 @@
       <c r="E3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2">
-        <v>721748392</v>
+      <c r="F3" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>11</v>
@@ -735,8 +757,8 @@
       <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
+      <c r="F4" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>12</v>
@@ -761,8 +783,8 @@
       <c r="E5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>38</v>
+      <c r="F5" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>12</v>
@@ -787,8 +809,8 @@
       <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>12</v>
+      <c r="F6" s="4" t="s">
+        <v>62</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>12</v>
@@ -813,8 +835,8 @@
       <c r="E7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F7" s="2">
-        <v>40765126291</v>
+      <c r="F7" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>15</v>
@@ -839,7 +861,7 @@
       <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="2" t="s">
@@ -865,7 +887,7 @@
       <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="2" t="s">
@@ -891,7 +913,7 @@
       <c r="E10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="2" t="s">
@@ -917,8 +939,8 @@
       <c r="E11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="2">
-        <v>765472891</v>
+      <c r="F11" s="4" t="s">
+        <v>59</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>21</v>
@@ -943,7 +965,7 @@
       <c r="E12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G12" s="2" t="s">

</xml_diff>

<commit_message>
deals values and descriptions can be changed too now
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\resurse CRM\Aplicatie licenta 2023 - 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227630B1-6E1F-4F3F-8C56-C6490979B721}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5639290-5F36-4E23-985E-B2B473B4D6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="2496" windowWidth="17280" windowHeight="8964" xr2:uid="{B355F5BB-8E75-495C-9323-1289A2C9F933}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B355F5BB-8E75-495C-9323-1289A2C9F933}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
   <si>
     <t>firstName</t>
   </si>
@@ -315,9 +315,6 @@
   </si>
   <si>
     <t>Robinson-Miller</t>
-  </si>
-  <si>
-    <t>prospect</t>
   </si>
   <si>
     <t>073916533</t>
@@ -750,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E4757DE-4F7A-4EC5-9011-0FEFE82C3666}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1069,7 +1066,7 @@
         <v>80</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>81</v>
@@ -1095,7 +1092,7 @@
         <v>85</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>86</v>
@@ -1121,13 +1118,13 @@
         <v>91</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>92</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
users can switch contact pipelineStatus
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\resurse CRM\Aplicatie licenta 2023 - 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5639290-5F36-4E23-985E-B2B473B4D6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3413DB18-BEFB-41F8-AB26-AA7FFBBDB370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B355F5BB-8E75-495C-9323-1289A2C9F933}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
   <si>
     <t>firstName</t>
   </si>
@@ -324,6 +324,9 @@
   </si>
   <si>
     <t>075919160</t>
+  </si>
+  <si>
+    <t>lead</t>
   </si>
 </sst>
 </file>
@@ -748,7 +751,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H14"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -838,7 +841,7 @@
         <v>34</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
- fixed task endpoit - fixed deals UI - fixed app crashing when too many emails are sent at once - team invite require valid email
</commit_message>
<xml_diff>
--- a/contacts.xlsx
+++ b/contacts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Desktop\resurse CRM\Aplicatie licenta 2023 - 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3413DB18-BEFB-41F8-AB26-AA7FFBBDB370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03EDCDF-CE75-4200-9224-22B541D58FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B355F5BB-8E75-495C-9323-1289A2C9F933}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="93">
   <si>
     <t>firstName</t>
   </si>
@@ -59,24 +59,12 @@
     <t>companyName</t>
   </si>
   <si>
-    <t>pipelineStatus</t>
-  </si>
-  <si>
     <t>FIMAX TRADING SRL</t>
   </si>
   <si>
-    <t>awd</t>
-  </si>
-  <si>
-    <t>awda</t>
-  </si>
-  <si>
     <t>SC PAPEX SRL</t>
   </si>
   <si>
-    <t>Erica</t>
-  </si>
-  <si>
     <t>Sava</t>
   </si>
   <si>
@@ -86,9 +74,6 @@
     <t>savaeric01@gmail.com</t>
   </si>
   <si>
-    <t>customer</t>
-  </si>
-  <si>
     <t>Robert</t>
   </si>
   <si>
@@ -104,9 +89,6 @@
     <t>pietroiurobert21@stud.ase.ro</t>
   </si>
   <si>
-    <t>George</t>
-  </si>
-  <si>
     <t>Robertutzu_cs12@yahoo.com</t>
   </si>
   <si>
@@ -263,9 +245,6 @@
     <t>0738443980</t>
   </si>
   <si>
-    <t>Bălăuță</t>
-  </si>
-  <si>
     <t>Christine</t>
   </si>
   <si>
@@ -305,9 +284,6 @@
     <t>Smith</t>
   </si>
   <si>
-    <t>Air cabin crew</t>
-  </si>
-  <si>
     <t>harrisvictoria@morgan-hernandez.com</t>
   </si>
   <si>
@@ -317,16 +293,28 @@
     <t>Robinson-Miller</t>
   </si>
   <si>
-    <t>073916533</t>
-  </si>
-  <si>
-    <t>079746980</t>
-  </si>
-  <si>
-    <t>075919160</t>
-  </si>
-  <si>
-    <t>lead</t>
+    <t>0739165331</t>
+  </si>
+  <si>
+    <t>0797469803</t>
+  </si>
+  <si>
+    <t>0759191609</t>
+  </si>
+  <si>
+    <t>Robert Adrian</t>
+  </si>
+  <si>
+    <t>Iancu</t>
+  </si>
+  <si>
+    <t>STR. ŞINCAI GHEORGHE nr. 34, MARAMUREŞ</t>
+  </si>
+  <si>
+    <t>Strada Drumul Urletei 768, Banesti</t>
+  </si>
+  <si>
+    <t>Eric</t>
   </si>
 </sst>
 </file>
@@ -358,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +362,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,13 +400,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -751,7 +750,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -760,7 +759,7 @@
     <col min="2" max="2" width="24.88671875" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="29.44140625" customWidth="1"/>
-    <col min="5" max="5" width="34" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" customWidth="1"/>
     <col min="6" max="6" width="29.44140625" customWidth="1"/>
     <col min="7" max="7" width="22.77734375" customWidth="1"/>
     <col min="8" max="8" width="21.5546875" customWidth="1"/>
@@ -788,347 +787,319 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="H1" s="6"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>92</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="F3" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>96</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>22</v>
+        <v>88</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="H9" s="7"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>74</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="H13" s="7"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="G14" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>16</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="H14" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>